<commit_message>
Update - Add ACTIVATION flag
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DE9347-CEE3-4EB1-AAA8-49845244F78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11865"/>
+    <workbookView xWindow="3495" yWindow="4440" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TOTAL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,14 +44,18 @@
   </si>
   <si>
     <t>TEST03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACTIVATION</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,12 +101,18 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -186,19 +197,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -212,6 +223,14 @@
       <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -258,7 +277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,9 +309,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,6 +361,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,77 +554,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.25" style="3" customWidth="1"/>
-    <col min="2" max="2" width="5.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="3"/>
+    <col min="2" max="2" width="10.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="5" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
         <v>20</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4">
         <v>50</v>
       </c>
-      <c r="C5" s="4">
+    </row>
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4">
+        <v>50</v>
+      </c>
+      <c r="D6" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4">
-        <v>100</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="D7" s="4">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -578,12 +657,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -592,12 +671,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>